<commit_message>
typo in excel spreadsheet!
</commit_message>
<xml_diff>
--- a/evorag_jul30_revision_results.xlsx
+++ b/evorag_jul30_revision_results.xlsx
@@ -201,12 +201,6 @@
     <t>6.019/0.50</t>
   </si>
   <si>
-    <t>0.042/ 0.0081</t>
-  </si>
-  <si>
-    <t>0.015/ 0.0073</t>
-  </si>
-  <si>
     <t>0.49/0.0091</t>
   </si>
   <si>
@@ -235,6 +229,12 @@
   </si>
   <si>
     <t>*why are the slopes always so different!</t>
+  </si>
+  <si>
+    <t>0.0041/ 0.078</t>
+  </si>
+  <si>
+    <t>-0.01/ 0.095</t>
   </si>
 </sst>
 </file>
@@ -317,7 +317,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -381,11 +381,14 @@
     <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,7 +694,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -723,19 +726,19 @@
         <v>5</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="24"/>
+      <c r="I1" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="23"/>
+      <c r="J1" s="24"/>
       <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
@@ -854,10 +857,10 @@
         <v>15</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G6" s="15">
         <v>-4.3221059999999999E-2</v>
@@ -886,8 +889,8 @@
       <c r="B7" s="13"/>
       <c r="C7" s="3"/>
       <c r="D7" s="16"/>
-      <c r="E7" s="24" t="s">
-        <v>72</v>
+      <c r="E7" s="23" t="s">
+        <v>70</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
@@ -1004,11 +1007,11 @@
       <c r="D12" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>62</v>
+      <c r="E12" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G12" s="17">
         <v>-3.5789660000000001E-2</v>
@@ -1151,10 +1154,10 @@
         <v>24</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G18" s="15">
         <v>-1.898041E-2</v>
@@ -1300,7 +1303,7 @@
         <v>30</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G24" s="15">
         <v>-9.7237190000000001E-2</v>

</xml_diff>